<commit_message>
[FEAT] Documento Unit testing finalizado
</commit_message>
<xml_diff>
--- a/UnitTesting/UnitTesting.xlsx
+++ b/UnitTesting/UnitTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcaf9\Documents\Escuela\10mo Semestre\PITE\BOSCH\bosch_eeprom\UnitTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4648818E-B5E1-4BBB-86BC-953D26AC4F05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E8398F2-AC83-4D47-8F7B-B59A916EC597}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{65163347-B616-477C-BCAF-62589AB2E79E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{65163347-B616-477C-BCAF-62589AB2E79E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,11 +30,83 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>Unit Testing</t>
+  </si>
+  <si>
+    <t>Test 1:</t>
+  </si>
+  <si>
+    <t>01.py</t>
+  </si>
+  <si>
+    <t>Test to find cnt file</t>
+  </si>
+  <si>
+    <t>Test 2:</t>
+  </si>
+  <si>
+    <t>Example.py</t>
+  </si>
+  <si>
+    <t>test to understand how XML trees work</t>
+  </si>
+  <si>
+    <t>pruebaexcel.py</t>
+  </si>
+  <si>
+    <t>Test 3:</t>
+  </si>
+  <si>
+    <t>Test 4:</t>
+  </si>
+  <si>
+    <t>pruebaCNT3.py</t>
+  </si>
+  <si>
+    <t>Test to order excel cells by values</t>
+  </si>
+  <si>
+    <t>Test to get data from a container</t>
+  </si>
+  <si>
+    <t>This tests were made for the libraries we used to learn how to work and manipulate them, the rest is pure logic.</t>
+  </si>
+  <si>
+    <t>Test 5:</t>
+  </si>
+  <si>
+    <t>logfiletest.py</t>
+  </si>
+  <si>
+    <t>test to create log files with content from a container</t>
+  </si>
+  <si>
+    <t>Test 6</t>
+  </si>
+  <si>
+    <t>valuesexcel.py</t>
+  </si>
+  <si>
+    <t>Test to save anything into a Excel file</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="36"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -61,8 +133,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -78,6 +156,363 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>63131</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>154781</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B91D50-7728-4CE8-AEF6-76391FF633E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="797720" y="1079183"/>
+          <a:ext cx="4849442" cy="2647473"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>547687</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>8928</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>485869</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>166144</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C5238C3-D4E9-4C34-B763-8E93D9C71233}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6131718" y="1080491"/>
+          <a:ext cx="4724495" cy="2657528"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>774061</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AD1E1CFB-3B4B-4139-82EF-FBC2C8BC68F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="793750" y="4572000"/>
+          <a:ext cx="4742811" cy="2857500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9294</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>2</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9294</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>79268</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C64B4F4-2BC3-4B25-ADC5-78C88F31855E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="799172" y="7620002"/>
+          <a:ext cx="4739268" cy="2681217"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28728</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>78829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagen 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69FDC67D-0AB7-4A4C-B9FC-276092DE09A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="789878" y="10593660"/>
+          <a:ext cx="4767996" cy="2680779"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>33654</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>84667</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7D1655A-9E9E-4F61-A019-BCCAC552C095}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="804333" y="12361333"/>
+          <a:ext cx="4859654" cy="2455334"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>169333</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>8763</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88670258-EC95-4ED4-AF99-3A795CD652AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6434667" y="12361333"/>
+          <a:ext cx="4995333" cy="2548762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9293</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>69114</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1F51BB5-17FF-4152-9E44-23E21661ACEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="789878" y="10593659"/>
+          <a:ext cx="4748561" cy="2671065"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,12 +812,133 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71ABB862-44F7-4357-8FDB-5C22A929CEC3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A126" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" t="s">
+        <v>18</v>
+      </c>
+      <c r="D57" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>17</v>
+      </c>
+      <c r="B89" t="s">
+        <v>15</v>
+      </c>
+      <c r="C89" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>